<commit_message>
Data provider concept in DD framework
</commit_message>
<xml_diff>
--- a/DataDrivenFramework/bin/com/excel/testdata/HalfEBayTestData.xlsx
+++ b/DataDrivenFramework/bin/com/excel/testdata/HalfEBayTestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>Firstname</t>
   </si>
@@ -40,6 +40,18 @@
   </si>
   <si>
     <t>padma@123</t>
+  </si>
+  <si>
+    <t>Somu</t>
+  </si>
+  <si>
+    <t>Ravi</t>
+  </si>
+  <si>
+    <t>Uma</t>
+  </si>
+  <si>
+    <t>S</t>
   </si>
 </sst>
 </file>
@@ -404,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,13 +458,61 @@
         <v>7</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="C3" r:id="rId3"/>
+    <hyperlink ref="C4" r:id="rId4"/>
+    <hyperlink ref="C5" r:id="rId5"/>
+    <hyperlink ref="D3" r:id="rId6"/>
+    <hyperlink ref="D4" r:id="rId7"/>
+    <hyperlink ref="D5" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
 

</xml_diff>